<commit_message>
etapa 1, 2, 3, 4 completa del sprint 1
</commit_message>
<xml_diff>
--- a/Etapa 1 - Inicio del Proyecto/Cronograma.xlsx
+++ b/Etapa 1 - Inicio del Proyecto/Cronograma.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Universidad\Agiles\Trabajos\Grupo3-2B_Workshop\Etapa 1 - Inicio del Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D0F80F-B912-47A1-BA0E-9ED5D851E116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41CDCC5-7788-4D97-AC94-122664B3F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E1F4E2F8-5766-42C9-8963-E217545A15CE}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="15375" windowHeight="7725" xr2:uid="{E1F4E2F8-5766-42C9-8963-E217545A15CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -239,13 +238,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DACD86-9A42-430B-818A-F86A7AB32E28}">
   <dimension ref="A2:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -578,54 +577,54 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="18">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" ht="18">
       <c r="A4" s="1"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="18">
       <c r="A5" s="1" t="s">
@@ -637,14 +636,14 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="18">
       <c r="A6" s="1" t="s">
@@ -656,14 +655,14 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="15.6">
       <c r="A7" s="3"/>
@@ -671,14 +670,14 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="18">
       <c r="A8" s="7" t="s">
@@ -762,16 +761,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
@@ -784,32 +773,27 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09795F8C-AB99-4F41-90D9-6342476FCAA8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="485955a5-5929-4e63-b593-5698b7bd71c0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1060,17 +1044,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="485955a5-5929-4e63-b593-5698b7bd71c0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F85D2AEF-9FF7-4B14-B46D-DA3D0C676AFE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5184A752-A329-4C36-BA0B-1A14FED79BB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8154b93f-f443-413d-9046-18733285ebd9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="485955a5-5929-4e63-b593-5698b7bd71c0"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1095,18 +1089,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5184A752-A329-4C36-BA0B-1A14FED79BB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F85D2AEF-9FF7-4B14-B46D-DA3D0C676AFE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8154b93f-f443-413d-9046-18733285ebd9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="485955a5-5929-4e63-b593-5698b7bd71c0"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>